<commit_message>
uses all data to train
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Idli rice</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Soya chunks</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>DATE</t>
@@ -631,7 +628,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -641,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BP2" sqref="BP2"/>
+    <sheetView tabSelected="1" topLeftCell="AU151" workbookViewId="0">
+      <selection activeCell="BA158" sqref="BA158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -652,19 +649,19 @@
   <sheetData>
     <row r="1" spans="1:68" ht="15">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -691,25 +688,25 @@
         <v>8</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>11</v>
@@ -718,28 +715,28 @@
         <v>12</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AE1" s="2" t="s">
         <v>13</v>
@@ -748,13 +745,13 @@
         <v>14</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AJ1" s="2" t="s">
         <v>15</v>
@@ -763,19 +760,19 @@
         <v>16</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AQ1" s="2" t="s">
         <v>17</v>
@@ -796,10 +793,10 @@
         <v>22</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AY1" s="2" t="s">
         <v>23</v>
@@ -808,13 +805,13 @@
         <v>24</v>
       </c>
       <c r="BA1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="BD1" s="2" t="s">
         <v>25</v>
@@ -823,16 +820,16 @@
         <v>26</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="BG1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="BH1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BJ1" s="2" t="s">
         <v>28</v>
@@ -844,7 +841,7 @@
         <v>30</v>
       </c>
       <c r="BM1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BN1" s="2" t="s">
         <v>31</v>
@@ -855,7 +852,7 @@
     </row>
     <row r="2" spans="1:68" ht="15">
       <c r="A2" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -32476,8 +32473,8 @@
       <c r="AZ157" s="3">
         <v>0</v>
       </c>
-      <c r="BA157" s="3" t="s">
-        <v>33</v>
+      <c r="BA157" s="3">
+        <v>1</v>
       </c>
       <c r="BB157" s="3">
         <v>0</v>

</xml_diff>